<commit_message>
Fixed formatting of About page
</commit_message>
<xml_diff>
--- a/static/background/Graphics.xlsx
+++ b/static/background/Graphics.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8160" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Home" sheetId="1" r:id="rId1"/>
+    <sheet name="Other" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -46,12 +47,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -68,10 +63,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,13 +614,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>46201</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>157099</xdr:rowOff>
+      <xdr:rowOff>170706</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>240758</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>164539</xdr:rowOff>
+      <xdr:rowOff>178146</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -635,7 +629,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1270844" y="3205099"/>
+          <a:off x="1270844" y="3218706"/>
           <a:ext cx="16727235" cy="2864940"/>
           <a:chOff x="3032256" y="3604515"/>
           <a:chExt cx="13492721" cy="2334351"/>
@@ -4484,36 +4478,2930 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>96488</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>115538</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>176894</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="96488" y="2136322"/>
+          <a:ext cx="19613336" cy="5660572"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>471415</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>173926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>494353</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>109685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="21300408">
+          <a:off x="6594629" y="6460426"/>
+          <a:ext cx="1247581" cy="1269259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>80480</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>185201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609392</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165489</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="17413902">
+          <a:off x="3171471" y="4346817"/>
+          <a:ext cx="1694788" cy="1753555"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>521169</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>172753</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304582</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>48674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2482707">
+          <a:off x="7869026" y="3792253"/>
+          <a:ext cx="1008056" cy="1018921"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>316717</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10168</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>557893</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>108710</xdr:colOff>
+      <xdr:colOff>257816</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>102449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2019147">
+          <a:off x="6439931" y="4582168"/>
+          <a:ext cx="1778064" cy="1806781"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>493563</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>108898</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584709</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>32328</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2784944">
+          <a:off x="4809243" y="4460968"/>
+          <a:ext cx="1256930" cy="1315789"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>396990</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>103804</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>537074</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>72918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:duotone>
+            <a:prstClr val="black"/>
+            <a:schemeClr val="accent1">
+              <a:tint val="45000"/>
+              <a:satMod val="400000"/>
+            </a:schemeClr>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="3311042">
+          <a:off x="7143172" y="3903158"/>
+          <a:ext cx="731114" cy="752405"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>505878</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>181826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>521289</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57697</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="3218842">
+          <a:off x="10318362" y="3214485"/>
+          <a:ext cx="1209371" cy="1240054"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476895</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>90549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>595825</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>90585</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="6845308">
+          <a:off x="9074824" y="4065620"/>
+          <a:ext cx="1905036" cy="1955894"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>256506</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>364083</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>63858</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="21201441">
+          <a:off x="8829006" y="2894678"/>
+          <a:ext cx="1332220" cy="1360180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>321929</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>182239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533352</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2876199">
+          <a:off x="2170386" y="3218746"/>
+          <a:ext cx="1413079" cy="1436066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>14074</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>175449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>513412</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>170924</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="3087095">
+          <a:off x="633398" y="3597446"/>
+          <a:ext cx="1709975" cy="1723981"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>190951</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>525175</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>151391</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1459402">
+          <a:off x="8151130" y="4705273"/>
+          <a:ext cx="946545" cy="970618"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>452395</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>183516</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>403559</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>186649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:duotone>
+            <a:prstClr val="black"/>
+            <a:schemeClr val="accent6">
+              <a:tint val="45000"/>
+              <a:satMod val="400000"/>
+            </a:schemeClr>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="4479154">
+          <a:off x="14550625" y="3978679"/>
+          <a:ext cx="1146133" cy="1175807"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>471449</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>79959</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>442803</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>155796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="745298">
+          <a:off x="13942520" y="2937459"/>
+          <a:ext cx="1195997" cy="1218837"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>454942</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>27278</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>586931</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>121730</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2395329">
+          <a:off x="12577669" y="4027778"/>
+          <a:ext cx="1950398" cy="1999452"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>393002</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>110324</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>139975</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>16999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20046509">
+          <a:off x="5242093" y="5634824"/>
+          <a:ext cx="1565382" cy="1621175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>496934</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>193424</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>168942</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1048979">
+          <a:off x="7770570" y="5666797"/>
+          <a:ext cx="1514899" cy="1550645"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>218953</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>46117</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>440514</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>186397</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1539349">
+          <a:off x="9310998" y="5951617"/>
+          <a:ext cx="1433834" cy="1473780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>72072</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>30645</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>563144</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="19007104">
+          <a:off x="12318501" y="2316645"/>
+          <a:ext cx="1715714" cy="1750071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>305567</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>146785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>463290</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>27652</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20837562">
+          <a:off x="3942385" y="5861785"/>
+          <a:ext cx="1369996" cy="1404867"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180399</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>168297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>340502</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="104" name="Picture 103"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+      <xdr:rowOff>51615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="57" name="Picture 56"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18" cstate="print">
+          <a:duotone>
+            <a:prstClr val="black"/>
+            <a:schemeClr val="accent6">
+              <a:tint val="45000"/>
+              <a:satMod val="400000"/>
+            </a:schemeClr>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1561995">
+          <a:off x="2604944" y="6073797"/>
+          <a:ext cx="1372376" cy="1407318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>295059</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>94636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>62195</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>137398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20069414">
+          <a:off x="1507332" y="6381136"/>
+          <a:ext cx="979408" cy="995262"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>75232</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>3534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>250356</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>89264</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8518072" y="0"/>
-          <a:ext cx="14246531" cy="7524751"/>
+          <a:off x="1893641" y="4956534"/>
+          <a:ext cx="1387397" cy="1419230"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>345436</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>232575</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>185529</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 59"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2026606">
+          <a:off x="10754900" y="5724912"/>
+          <a:ext cx="1111782" cy="1128117"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>21270</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>162316</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>414954</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28632</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20933744">
+          <a:off x="11537861" y="6258316"/>
+          <a:ext cx="999820" cy="1009316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>391367</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>49178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>146562</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>88479</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 61"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1651246">
+          <a:off x="11907958" y="5383178"/>
+          <a:ext cx="967468" cy="991801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>410981</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>77434</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>16330</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>154164</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 62"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent3">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20602081">
+          <a:off x="14352117" y="5220934"/>
+          <a:ext cx="817622" cy="838730"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>351839</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>50252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>238978</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>35369</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2308505">
+          <a:off x="13080703" y="5955752"/>
+          <a:ext cx="1099411" cy="1128117"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>570421</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>189947</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>174138</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180892</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 64"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="19510812">
+          <a:off x="15266135" y="4952447"/>
+          <a:ext cx="2053003" cy="2086445"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161038</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>11755</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>99351</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>176493</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 65"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="3959280">
+          <a:off x="14118848" y="6091081"/>
+          <a:ext cx="1117238" cy="1150586"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>299670</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>160030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>495311</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>72096</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 66"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1795217">
+          <a:off x="16832349" y="4160530"/>
+          <a:ext cx="1420283" cy="1436066"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>584567</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>175009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>407132</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>141694</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Picture 67"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="329666">
+          <a:off x="5483138" y="3223009"/>
+          <a:ext cx="1659530" cy="1681185"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>559043</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>111959</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>193480</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>26650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Picture 69"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="6717964">
+          <a:off x="566120" y="5248382"/>
+          <a:ext cx="1438691" cy="1452846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>310636</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>4737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>436544</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>2648</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Picture 70"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="2884475">
+          <a:off x="15628242" y="3614667"/>
+          <a:ext cx="1331411" cy="1350551"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>507259</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>168705</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>487329</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>56497</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 71"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1174184">
+          <a:off x="10916723" y="4359705"/>
+          <a:ext cx="1204713" cy="1221292"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>314074</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>396670</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>177358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 72"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16917767">
+          <a:off x="16857833" y="3494021"/>
+          <a:ext cx="672757" cy="694917"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88463</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>87561</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>413504</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>93230</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 73"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3762392" y="3516561"/>
+          <a:ext cx="937362" cy="958169"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>385385</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>77648</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>26536</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9478</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="75" name="Picture 74"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="1340226">
+          <a:off x="4671635" y="3506648"/>
+          <a:ext cx="865794" cy="884330"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203366</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>94065</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9401</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>119490</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="76" name="Picture 75" descr="Database management system Computer Icons Microsoft SQL Server ..."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33" cstate="print">
+          <a:biLevel thresh="75000"/>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8163545" y="4094565"/>
+          <a:ext cx="418356" cy="406425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>390864</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>36879</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>78180</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>173918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="77" name="Picture 76" descr="Download Free Icons Python Programming Computer Social Tutorial ..."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34" cstate="print">
+          <a:biLevel thresh="75000"/>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9575685" y="4608879"/>
+          <a:ext cx="911959" cy="899039"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>453313</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>65383</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>496534</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>146704</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="78" name="Picture 77"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20755482">
+          <a:off x="5964206" y="3684883"/>
+          <a:ext cx="655542" cy="652821"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276745</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41464</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>344448</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="79" name="Picture 78"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6944245" y="5184964"/>
+          <a:ext cx="673839" cy="720535"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>45520</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>436665</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>175908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="80" name="Picture 79"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12168247" y="5687785"/>
+          <a:ext cx="391145" cy="393623"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>426102</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>122786</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>333252</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>89567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="81" name="Picture 80"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1032238" y="5647286"/>
+          <a:ext cx="513287" cy="538281"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>268261</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>147030</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>189016</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>22354</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Picture 81"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5166832" y="4909530"/>
+          <a:ext cx="533077" cy="446824"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>527115</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>52099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>191828</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>65062</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="83" name="Picture 82"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8487294" y="5005099"/>
+          <a:ext cx="277034" cy="393963"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>88322</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>97719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>50220</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>173918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="84" name="Picture 83"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16008679" y="4098219"/>
+          <a:ext cx="574220" cy="457199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>594829</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>102651</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>80158</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>51455</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="85" name="Picture 84"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3656436" y="4865151"/>
+          <a:ext cx="709972" cy="710804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>371994</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>37848</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>158895</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>146705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="86" name="Picture 85"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20832289">
+          <a:off x="4045923" y="3847848"/>
+          <a:ext cx="399222" cy="299357"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>607099</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>68036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>197179</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>121501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="87" name="Picture 86"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15915135" y="5592536"/>
+          <a:ext cx="814723" cy="815465"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>143</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>175395</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>376149</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>147067</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="88" name="Picture 87" descr="Wisconsin Badgers - Wikipedia"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45" cstate="print">
+          <a:biLevel thresh="75000"/>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="411096">
+          <a:off x="4898714" y="3794895"/>
+          <a:ext cx="376006" cy="352672"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>539215</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107758</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>203849</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>991</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="89" name="Picture 88"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="591446">
+          <a:off x="17071894" y="3727258"/>
+          <a:ext cx="276955" cy="274233"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>43122</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>149676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>376125</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>94207</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="90" name="Picture 89"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14590395" y="5483676"/>
+          <a:ext cx="333003" cy="325531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>440029</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190342</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>523751</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>8200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="91" name="Picture 90"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId48" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13168893" y="4571842"/>
+          <a:ext cx="689858" cy="770358"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>417614</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>190497</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>243443</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>12966</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="92" name="Picture 91"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8297387" y="6095997"/>
+          <a:ext cx="431965" cy="584469"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>554009</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>27213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>450187</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>177213</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="93" name="Picture 92"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2372418" y="5361213"/>
+          <a:ext cx="502314" cy="531000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>248885</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>59569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>546523</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>31741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="94" name="Picture 93"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51" cstate="print">
+          <a:duotone>
+            <a:prstClr val="black"/>
+            <a:schemeClr val="accent6">
+              <a:tint val="45000"/>
+              <a:satMod val="400000"/>
+            </a:schemeClr>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="20916044">
+          <a:off x="11882992" y="3869569"/>
+          <a:ext cx="909960" cy="924672"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>325086</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>187524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>83423</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>51451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="95" name="Picture 94"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11346872" y="4759524"/>
+          <a:ext cx="370658" cy="435427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>151239</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>160099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>17567</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>58579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="96" name="Picture 95"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="523443">
+          <a:off x="14846953" y="4351099"/>
+          <a:ext cx="478650" cy="469980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>143297</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>43654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>66552</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>27212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="97" name="Picture 96"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17288297" y="4615654"/>
+          <a:ext cx="535576" cy="555058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>538602</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>154337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>278940</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>154493</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="98" name="Picture 97"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12172709" y="4154837"/>
+          <a:ext cx="352660" cy="381156"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>52939</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>83849</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>367039</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>130886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="132" name="Picture 131"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="19820496">
+          <a:off x="17197939" y="5608349"/>
+          <a:ext cx="1538743" cy="1571037"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4529,16 +7417,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>86591</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>106089</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>51955</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>173181</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>36816</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4555,8 +7443,101 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="606137" y="848591"/>
+          <a:off x="51955" y="969818"/>
           <a:ext cx="21335999" cy="8591998"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>272142</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>421821</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 63"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="1922" t="29058" r="7051" b="801"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="272142" y="1986642"/>
+          <a:ext cx="15457715" cy="4762501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>74102</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95917</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>305690</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>5039</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 64"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent5">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="19820496">
+          <a:off x="14769816" y="5048917"/>
+          <a:ext cx="843910" cy="861622"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4833,8 +7814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AG9:AX24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH23" sqref="AH23"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4868,20 +7849,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
-  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <webPublishItems count="1">
-    <webPublishItem id="24072" divId="Graphics_24072" sourceType="sheet" destinationFile="C:\Users\klausa\Desktop\Projects\DataScience\blog\static\background\Graphics.htm"/>
-  </webPublishItems>
 </worksheet>
 </file>
 
@@ -4901,4 +7876,22 @@
     <webPublishItem id="24057" divId="Graphics_24057" sourceType="sheet" destinationFile="C:\Users\klausa\Desktop\Projects\DataScience\blog\static\background\Graphics.htm"/>
   </webPublishItems>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <webPublishItems count="1">
+    <webPublishItem id="11190" divId="Graphics_11190" sourceType="sheet" destinationFile="C:\Users\klausa\Desktop\Projects\DataScience\blog\static\background\Graphics.htm"/>
+  </webPublishItems>
+</worksheet>
 </file>
</xml_diff>